<commit_message>
Correction to transportation files for aviation (remove international non-EU)
</commit_message>
<xml_diff>
--- a/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
+++ b/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\SYFAFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F781F-A5C0-4D19-893F-DECA34703388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91CDC78-59A8-4164-BC5C-52DC15BA480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="742" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="742" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2786,10 +2786,10 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="139.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="139.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2853,7 +2853,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="87">
+    <row r="14" spans="1:5" ht="120">
       <c r="B14" s="47" t="s">
         <v>10</v>
       </c>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="43.5">
+    <row r="20" spans="1:5" ht="60">
       <c r="B20" s="47" t="s">
         <v>14</v>
       </c>
@@ -3026,13 +3026,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="8" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -3502,12 +3502,12 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1" s="86" t="s">
         <v>179</v>
       </c>
@@ -7023,13 +7023,12 @@
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.1796875"/>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1" s="86" t="s">
         <v>174</v>
       </c>
@@ -10564,20 +10563,20 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
-    <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="42.7265625" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -10860,7 +10859,7 @@
       </c>
       <c r="I13" s="60"/>
     </row>
-    <row r="14" spans="1:10" ht="43.5">
+    <row r="14" spans="1:10" ht="45">
       <c r="A14" s="21" t="s">
         <v>39</v>
       </c>
@@ -11933,14 +11932,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" customWidth="1"/>
-    <col min="7" max="7" width="41.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="41.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12279,17 +12278,17 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.54296875" customWidth="1"/>
-    <col min="8" max="9" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
+    <col min="8" max="9" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12644,13 +12643,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
-    <col min="8" max="9" width="19.453125" customWidth="1"/>
+    <col min="8" max="9" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12963,20 +12962,20 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="A9:H29"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="8" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="5" t="s">
         <v>104</v>
       </c>
@@ -13081,8 +13080,8 @@
         <v>0</v>
       </c>
       <c r="E4" s="73">
-        <f>'Aviation Calculations'!E4</f>
-        <v>6.0269145731933641E-4</v>
+        <f>AVERAGE('Aviation Calculations'!E5:E6)</f>
+        <v>3.7297762719289314E-4</v>
       </c>
       <c r="F4" s="73">
         <v>0</v>
@@ -13295,20 +13294,20 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="8" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="5" t="s">
         <v>105</v>
       </c>
@@ -13412,8 +13411,8 @@
         <v>0</v>
       </c>
       <c r="E4" s="73">
-        <f>'Aviation Calculations'!E8</f>
-        <v>1.6207022383086511E-4</v>
+        <f>'Aviation Calculations'!E9</f>
+        <v>7.1350079212815194E-5</v>
       </c>
       <c r="F4" s="73">
         <v>0</v>
@@ -13686,15 +13685,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
@@ -13703,6 +13693,15 @@
     <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13935,20 +13934,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF912DF3-EA4C-4211-B7E9-EA25E2A94769}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D632F66-03C4-44FF-9808-B31E7AA18D4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
     <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF912DF3-EA4C-4211-B7E9-EA25E2A94769}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Re-correct aircraft transportation files
</commit_message>
<xml_diff>
--- a/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
+++ b/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\SYFAFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91CDC78-59A8-4164-BC5C-52DC15BA480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D3A52D-FAC3-4066-9A1B-FF738C70076D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="742" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5880" windowWidth="38640" windowHeight="21120" tabRatio="742" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2786,10 +2786,10 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="139.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="139.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2853,7 +2853,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="120">
+    <row r="14" spans="1:5" ht="87">
       <c r="B14" s="47" t="s">
         <v>10</v>
       </c>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="60">
+    <row r="20" spans="1:5" ht="43.5">
       <c r="B20" s="47" t="s">
         <v>14</v>
       </c>
@@ -3026,13 +3026,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="8" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="8" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -3502,12 +3502,12 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="86" t="s">
         <v>179</v>
       </c>
@@ -7023,12 +7023,12 @@
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="86" t="s">
         <v>174</v>
       </c>
@@ -10563,20 +10563,20 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1"/>
+    <col min="7" max="7" width="42.7265625" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -10859,7 +10859,7 @@
       </c>
       <c r="I13" s="60"/>
     </row>
-    <row r="14" spans="1:10" ht="45">
+    <row r="14" spans="1:10" ht="43.5">
       <c r="A14" s="21" t="s">
         <v>39</v>
       </c>
@@ -11932,14 +11932,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="41.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" customWidth="1"/>
+    <col min="7" max="7" width="41.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12278,17 +12278,17 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
-    <col min="8" max="9" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42.54296875" customWidth="1"/>
+    <col min="8" max="9" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12643,13 +12643,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
-    <col min="8" max="9" width="19.42578125" customWidth="1"/>
+    <col min="8" max="9" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12961,21 +12961,21 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="8" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="8" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="29">
       <c r="A1" s="5" t="s">
         <v>104</v>
       </c>
@@ -13080,8 +13080,8 @@
         <v>0</v>
       </c>
       <c r="E4" s="73">
-        <f>AVERAGE('Aviation Calculations'!E5:E6)</f>
-        <v>3.7297762719289314E-4</v>
+        <f>'Aviation Calculations'!E5</f>
+        <v>2.4082446227065575E-4</v>
       </c>
       <c r="F4" s="73">
         <v>0</v>
@@ -13294,20 +13294,20 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="8" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="8" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="29">
       <c r="A1" s="5" t="s">
         <v>105</v>
       </c>
@@ -13685,26 +13685,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4a12692b057bc30d68596ac87c75a308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4dd464ebbb7361a2027b4bc4be8d527a" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -13933,26 +13913,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D632F66-03C4-44FF-9808-B31E7AA18D4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF912DF3-EA4C-4211-B7E9-EA25E2A94769}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE28452B-5587-40CC-A9EE-4AAF8A3A964E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13969,4 +13950,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF912DF3-EA4C-4211-B7E9-EA25E2A94769}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D632F66-03C4-44FF-9808-B31E7AA18D4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to BAADTbVT file to add multiplier on LDV and HDV freight distance traveled
</commit_message>
<xml_diff>
--- a/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
+++ b/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\SYFAFE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\trans\SYFAFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D3A52D-FAC3-4066-9A1B-FF738C70076D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFF9753-D5A5-44D6-BB13-5C4D3311A67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5880" windowWidth="38640" windowHeight="21120" tabRatio="742" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="35220" yWindow="1935" windowWidth="21600" windowHeight="12645" tabRatio="742" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2786,10 +2786,10 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="139.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="139.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2853,7 +2853,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="87">
+    <row r="14" spans="1:5" ht="120">
       <c r="B14" s="47" t="s">
         <v>10</v>
       </c>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="43.5">
+    <row r="20" spans="1:5" ht="60">
       <c r="B20" s="47" t="s">
         <v>14</v>
       </c>
@@ -3026,13 +3026,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="8" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -3502,12 +3502,12 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1" s="86" t="s">
         <v>179</v>
       </c>
@@ -7023,12 +7023,12 @@
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1" s="86" t="s">
         <v>174</v>
       </c>
@@ -10561,22 +10561,24 @@
   </sheetPr>
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
-    <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="42.7265625" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -10859,7 +10861,7 @@
       </c>
       <c r="I13" s="60"/>
     </row>
-    <row r="14" spans="1:10" ht="43.5">
+    <row r="14" spans="1:10" ht="45">
       <c r="A14" s="21" t="s">
         <v>39</v>
       </c>
@@ -11018,7 +11020,7 @@
         <v>5842331988.5945225</v>
       </c>
       <c r="E19" s="54">
-        <f t="shared" si="4"/>
+        <f>D19/C60</f>
         <v>1.1619869328143087E-3</v>
       </c>
       <c r="G19" s="61" t="s">
@@ -11702,7 +11704,7 @@
         <v>126.70081146560065</v>
       </c>
       <c r="C60" s="50">
-        <f t="shared" si="11"/>
+        <f>B60*$G$10</f>
         <v>5027880971470.5771</v>
       </c>
       <c r="E60" s="50"/>
@@ -11932,14 +11934,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" customWidth="1"/>
-    <col min="7" max="7" width="41.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="41.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12281,14 +12283,14 @@
       <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.54296875" customWidth="1"/>
-    <col min="8" max="9" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
+    <col min="8" max="9" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12643,13 +12645,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
-    <col min="8" max="9" width="19.453125" customWidth="1"/>
+    <col min="8" max="9" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12961,21 +12963,21 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="8" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="5" t="s">
         <v>104</v>
       </c>
@@ -13298,16 +13300,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="8" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="5" t="s">
         <v>105</v>
       </c>
@@ -13914,15 +13916,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
@@ -13931,6 +13924,15 @@
     <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13953,14 +13955,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF912DF3-EA4C-4211-B7E9-EA25E2A94769}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D632F66-03C4-44FF-9808-B31E7AA18D4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -13969,4 +13963,12 @@
     <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF912DF3-EA4C-4211-B7E9-EA25E2A94769}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>